<commit_message>
Some scuffed part 3 analysis
</commit_message>
<xml_diff>
--- a/faraday/data/flint_dispersion.xlsx
+++ b/faraday/data/flint_dispersion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jackson\physics_387\faraday\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2193CD2-F86A-433E-84B2-EE6178C604B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CE6ACB-5D0D-4497-8E9B-58057E53A757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6916B59A-5344-41CF-A421-9E989B887428}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{6916B59A-5344-41CF-A421-9E989B887428}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,7 +396,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>